<commit_message>
Commit multiple changes for restructuring folder - 23 Sept
</commit_message>
<xml_diff>
--- a/src/steffs_pharmacy/invoices.xlsx
+++ b/src/steffs_pharmacy/invoices.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
@@ -865,6 +865,48 @@
         <v>15</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>SP23092022121400</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>100</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>PANADOL STRIP 10</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>SP23092022121400</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>101</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>PANADOL STRIP 20</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" t="n">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>